<commit_message>
Changes to be committed: 	modified:   docs/report-generator/092825-api-calls.xlsx 	deleted:    docs/report-generator/~$092825-api-calls.xlsx 	modified:   excel_data/vast_data_final_20250929_070753.xlsx 	deleted:    excel_data/~$vast_data_final_20250929_070753.xlsx
</commit_message>
<xml_diff>
--- a/docs/report-generator/092825-api-calls.xlsx
+++ b/docs/report-generator/092825-api-calls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.stamps/Documents/as-built-report/ps-deploy-report/docs/report-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277D2414-2A58-E74C-8AD6-A40F5133D5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F4366-A0DB-D942-9AF3-4EE92BB93ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="760" windowWidth="26440" windowHeight="21580" xr2:uid="{5D9104DC-D0A5-A54E-927F-9586B89AC5B0}"/>
+    <workbookView xWindow="2380" yWindow="5000" windowWidth="26440" windowHeight="21580" xr2:uid="{5D9104DC-D0A5-A54E-927F-9586B89AC5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="API-Summary" sheetId="17" r:id="rId1"/>

</xml_diff>